<commit_message>
agregado subtotal, iva y total en facutras
</commit_message>
<xml_diff>
--- a/Plantilla/TemplateFacturas.xlsx
+++ b/Plantilla/TemplateFacturas.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stambour\OneDrive - DXC Production\Personal\Desarrollo\Repos\Cinderella\Plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="25" documentId="11_D91601F0DED5E7358A217455409C7F49F501C076" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{D5C3CBA1-A980-4214-B78B-329D616DFEFB}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10485"/>
+    <workbookView xWindow="3735" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Facturas" sheetId="2" r:id="rId1"/>
@@ -28,14 +29,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Sucursal:</t>
   </si>
   <si>
-    <t>Monto</t>
-  </si>
-  <si>
     <t>Número</t>
   </si>
   <si>
@@ -61,15 +59,24 @@
   </si>
   <si>
     <t>Fecha</t>
+  </si>
+  <si>
+    <t>Sub Total</t>
+  </si>
+  <si>
+    <t>IVA</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;\ #,##0.00"/>
     <numFmt numFmtId="166" formatCode="0_ ;\-0\ "/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
@@ -140,28 +147,24 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -181,6 +184,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -461,84 +468,98 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="21" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="16" customWidth="1"/>
-    <col min="3" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="8" width="15.7109375" style="22" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" style="9" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" style="22" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="17" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="12" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="9" width="15.7109375" style="18" customWidth="1"/>
+    <col min="10" max="12" width="15.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="13"/>
+      <c r="C1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="E3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="F3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="G3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="H3" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="I3" s="19" t="s">
         <v>8</v>
-      </c>
-      <c r="H3" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>1</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>10</v>
       </c>
+      <c r="K3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="11"/>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="23"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
       <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="12"/>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
       <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>